<commit_message>
Commit before changing GetMoreForIntId
</commit_message>
<xml_diff>
--- a/asp.net core api checklist.xlsx
+++ b/asp.net core api checklist.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhilippPrivate\Documents\Visual Studio 2017\Projects\Fittify\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS 2017 Projects\Fittify\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20805" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Api Status Codes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Datamodel</t>
   </si>
@@ -108,14 +109,146 @@
   </si>
   <si>
     <t>HATEOES</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <r>
+      <t>return Ok()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ← Http status code 200</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>return Created()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ← Http status code 201</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>return NoContent();</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ← Http status code 204</t>
+    </r>
+  </si>
+  <si>
+    <t>Client Error:</t>
+  </si>
+  <si>
+    <r>
+      <t>return BadRequest();</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ← Http status code 400</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>return Unauthorized();</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ← Http status code 401</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>return NotFound();</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ← Http status code 404</t>
+    </r>
+  </si>
+  <si>
+    <t>Do!</t>
+  </si>
+  <si>
+    <t>ApiVersioning</t>
+  </si>
+  <si>
+    <t>unprocessable entity</t>
+  </si>
+  <si>
+    <t>ToDo</t>
+  </si>
+  <si>
+    <t>Route not found!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -144,8 +277,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,6 +681,9 @@
       <c r="B13" t="s">
         <v>23</v>
       </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -597,6 +740,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
@@ -605,4 +753,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>422</v>
+      </c>
+      <c r="L12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Improved Get and Post, still working on Patch
</commit_message>
<xml_diff>
--- a/asp.net core api checklist.xlsx
+++ b/asp.net core api checklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Datamodel</t>
   </si>
@@ -226,6 +226,27 @@
   </si>
   <si>
     <t>Route not found!</t>
+  </si>
+  <si>
+    <t>Heavily changed controller</t>
+  </si>
+  <si>
+    <t>GetById</t>
+  </si>
+  <si>
+    <t>GetAll</t>
+  </si>
+  <si>
+    <t>GetByRangeOfId</t>
+  </si>
+  <si>
+    <t>Patch</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -566,91 +587,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:K9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>47</v>
+      </c>
+      <c r="P7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -658,7 +764,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -666,7 +772,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -674,7 +780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -685,7 +791,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -693,7 +799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -701,7 +807,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -759,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Json PATCH is now working
</commit_message>
<xml_diff>
--- a/asp.net core api checklist.xlsx
+++ b/asp.net core api checklist.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="8505"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17535" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Api Status Codes" sheetId="2" r:id="rId2"/>
+    <sheet name="ToDo" sheetId="1" r:id="rId1"/>
+    <sheet name="Routing Rules" sheetId="3" r:id="rId2"/>
+    <sheet name="Api Status Codes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
   <si>
     <t>Datamodel</t>
   </si>
@@ -213,9 +214,6 @@
     </r>
   </si>
   <si>
-    <t>Do!</t>
-  </si>
-  <si>
     <t>ApiVersioning</t>
   </si>
   <si>
@@ -240,6 +238,9 @@
     <t>GetByRangeOfId</t>
   </si>
   <si>
+    <t>Post</t>
+  </si>
+  <si>
     <t>Patch</t>
   </si>
   <si>
@@ -247,6 +248,21 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>all lowercase, separated by hyphens "-"</t>
+  </si>
+  <si>
+    <t>/pluralized</t>
+  </si>
+  <si>
+    <t>/pluralized/{id}</t>
+  </si>
+  <si>
+    <t>/range/pluralized</t>
+  </si>
+  <si>
+    <t>/pluralized/new</t>
   </si>
 </sst>
 </file>
@@ -589,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,13 +626,13 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
@@ -753,7 +769,7 @@
         <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -763,6 +779,21 @@
       <c r="B10" t="s">
         <v>23</v>
       </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -771,6 +802,15 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -788,7 +828,13 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -848,7 +894,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -862,6 +908,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="33.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:L15"/>
   <sheetViews>
@@ -920,15 +1030,15 @@
         <v>422</v>
       </c>
       <c r="L12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" t="s">
         <v>39</v>
-      </c>
-      <c r="L15" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>